<commit_message>
changes in IP-address plan
</commit_message>
<xml_diff>
--- a/labs/lab04 Planning/export_zip/LAB04.xlsx
+++ b/labs/lab04 Planning/export_zip/LAB04.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artys\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\otus-network-engineer\labs\lab04 Planning\export_zip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDC31DC8-2EA3-4FE9-A667-58FB1374F04D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34800B3D-D7DF-49AB-AC46-F9CBB7B38DB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CA3414E2-F7C9-42D3-81A5-4C381A8414F5}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{CA3414E2-F7C9-42D3-81A5-4C381A8414F5}"/>
   </bookViews>
   <sheets>
     <sheet name="IP" sheetId="1" r:id="rId1"/>
@@ -22,12 +22,18 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="270">
   <si>
     <t>Москва</t>
   </si>
@@ -476,12 +482,6 @@
     <t>to LMS-R21.e0/0</t>
   </si>
   <si>
-    <t>10.0.254.21</t>
-  </si>
-  <si>
-    <t>10.0.254.20</t>
-  </si>
-  <si>
     <t>to KTN-R22.e0/0</t>
   </si>
   <si>
@@ -503,12 +503,6 @@
     <t>192.168.21.1</t>
   </si>
   <si>
-    <t>10.0.254.41</t>
-  </si>
-  <si>
-    <t>10.0.254.40</t>
-  </si>
-  <si>
     <t>10.0.254.42</t>
   </si>
   <si>
@@ -674,12 +668,6 @@
     <t>65-78</t>
   </si>
   <si>
-    <t>10.0.254.0/28</t>
-  </si>
-  <si>
-    <t>1-14</t>
-  </si>
-  <si>
     <t>10.0.254.138</t>
   </si>
   <si>
@@ -791,30 +779,12 @@
     <t>10.0.254.8</t>
   </si>
   <si>
-    <t>10.0.254.16/29</t>
-  </si>
-  <si>
-    <t>17-22</t>
-  </si>
-  <si>
-    <t>25-30</t>
-  </si>
-  <si>
-    <t>10.0.254.24/29</t>
-  </si>
-  <si>
     <t>10.0.254.18</t>
   </si>
   <si>
     <t>10.0.254.19</t>
   </si>
   <si>
-    <t>10.0.254.26</t>
-  </si>
-  <si>
-    <t>10.0.254.27</t>
-  </si>
-  <si>
     <t>10.0.254.48/28</t>
   </si>
   <si>
@@ -822,6 +792,57 @@
   </si>
   <si>
     <t>CKD-SW29</t>
+  </si>
+  <si>
+    <t>10.0.254.32/29</t>
+  </si>
+  <si>
+    <t>33-38</t>
+  </si>
+  <si>
+    <t>10.0.254.0/27</t>
+  </si>
+  <si>
+    <t>10.0.254.40/29</t>
+  </si>
+  <si>
+    <t>41-46</t>
+  </si>
+  <si>
+    <t>1-30</t>
+  </si>
+  <si>
+    <t>10.0.254.34</t>
+  </si>
+  <si>
+    <t>10.0.254.15</t>
+  </si>
+  <si>
+    <t>10.0.254.35</t>
+  </si>
+  <si>
+    <t>10.0.254.36</t>
+  </si>
+  <si>
+    <t>10.0.254.14</t>
+  </si>
+  <si>
+    <t>10.0.254.17</t>
+  </si>
+  <si>
+    <t>10.0.254.16</t>
+  </si>
+  <si>
+    <t>10.0.254.37</t>
+  </si>
+  <si>
+    <t>e1/0</t>
+  </si>
+  <si>
+    <t>to R15.e1/0</t>
+  </si>
+  <si>
+    <t>to R14.e1/0</t>
   </si>
 </sst>
 </file>
@@ -1221,107 +1242,11 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1330,6 +1255,123 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1340,27 +1382,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1683,10 +1704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03742B99-8A41-4105-910E-954797F66359}">
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98:G100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,19 +1728,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>250</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="50" t="s">
-        <v>251</v>
-      </c>
-      <c r="I1" s="50"/>
+      <c r="A1" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="I1" s="27"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1744,21 +1765,21 @@
         <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>215</v>
-      </c>
-      <c r="I2" s="48" t="s">
-        <v>216</v>
+        <v>255</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="49" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>115</v>
@@ -1770,7 +1791,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="A4" s="49"/>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1787,12 +1808,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
+      <c r="A5" s="49"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>115</v>
@@ -1800,11 +1821,11 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1821,46 +1842,46 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>122</v>
+        <v>267</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>21</v>
-      </c>
+      <c r="A8" s="49"/>
       <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>115</v>
+        <v>61</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
-        <v>136</v>
-      </c>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+      <c r="A9" s="49" t="s">
+        <v>21</v>
+      </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>129</v>
+        <v>247</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>115</v>
@@ -1868,16 +1889,16 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>259</v>
+        <v>129</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>115</v>
@@ -1885,16 +1906,16 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>132</v>
+        <v>249</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>115</v>
@@ -1902,249 +1923,249 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>97</v>
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="49"/>
+      <c r="B13" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="49"/>
+      <c r="B14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1">
-        <v>10</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1">
-        <v>11</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1">
+        <v>10</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="49"/>
+      <c r="B16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>11</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="49"/>
+      <c r="B17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
         <v>55</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="1" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="49"/>
+      <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>122</v>
+      <c r="C18" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="49"/>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="49"/>
+      <c r="B20" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1">
-        <v>10</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="17"/>
-      <c r="B20" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1">
-        <v>11</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="17"/>
-      <c r="B21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1">
+        <v>10</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="49"/>
+      <c r="B22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1">
+        <v>11</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="49"/>
+      <c r="B23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1">
         <v>55</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="1" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="49"/>
+      <c r="B24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="17"/>
-      <c r="B24" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>122</v>
+      <c r="D24" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="G24" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
-        <v>24</v>
-      </c>
+      <c r="A25" s="49"/>
       <c r="B25" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>115</v>
@@ -2152,16 +2173,16 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="17"/>
+      <c r="A26" s="49"/>
       <c r="B26" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>122</v>
@@ -2171,14 +2192,14 @@
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
-        <v>25</v>
+      <c r="A27" s="49" t="s">
+        <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>115</v>
@@ -2186,16 +2207,16 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="17"/>
+      <c r="A28" s="49"/>
       <c r="B28" s="1" t="s">
         <v>138</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>122</v>
@@ -2205,56 +2226,48 @@
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>26</v>
+      <c r="A29" s="49" t="s">
+        <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>68</v>
+        <v>134</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F29" s="1">
-        <v>55</v>
-      </c>
-      <c r="G29" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="A30" s="49"/>
       <c r="B30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="1">
-        <v>55</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>71</v>
@@ -2269,13 +2282,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>71</v>
@@ -2290,110 +2303,112 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="F33" s="1">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="1">
+        <v>55</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="1">
+        <v>10</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F36" s="1">
         <v>11</v>
       </c>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="50" t="s">
-        <v>251</v>
-      </c>
-      <c r="I35" s="50"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
+      <c r="B37" s="37"/>
+      <c r="C37" s="37"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="I37" s="27"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="H36" t="s">
-        <v>213</v>
-      </c>
-      <c r="I36" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="4" t="s">
-        <v>8</v>
-      </c>
       <c r="C38" s="4" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>115</v>
@@ -2401,16 +2416,22 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
+      </c>
+      <c r="H38" t="s">
+        <v>209</v>
+      </c>
+      <c r="I38" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>115</v>
@@ -2418,186 +2439,186 @@
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
+      <c r="A40" s="50"/>
       <c r="B40" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>122</v>
+        <v>8</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="G40" s="4" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="46" t="s">
-        <v>17</v>
-      </c>
+      <c r="A41" s="50"/>
       <c r="B41" s="4" t="s">
-        <v>239</v>
+        <v>9</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4" t="s">
-        <v>245</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="64"/>
+      <c r="A42" s="50"/>
       <c r="B42" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>97</v>
+        <v>138</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="4" t="s">
-        <v>246</v>
-      </c>
+      <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="64"/>
+      <c r="A43" s="32" t="s">
+        <v>17</v>
+      </c>
       <c r="B43" s="4" t="s">
-        <v>7</v>
+        <v>233</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="48"/>
+      <c r="B44" s="4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="64"/>
-      <c r="B44" s="4" t="s">
-        <v>200</v>
-      </c>
       <c r="C44" s="4" t="s">
-        <v>63</v>
+        <v>236</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
+      <c r="A45" s="48"/>
       <c r="B45" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="D45" s="15" t="s">
-        <v>122</v>
+        <v>7</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="G45" s="4" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="46" t="s">
-        <v>18</v>
-      </c>
+      <c r="A46" s="48"/>
       <c r="B46" s="4" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>243</v>
+        <v>63</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="64"/>
+      <c r="A47" s="33"/>
       <c r="B47" s="4" t="s">
-        <v>240</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>97</v>
+        <v>138</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
-      <c r="G47" s="4" t="s">
-        <v>246</v>
-      </c>
+      <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="64"/>
+      <c r="A48" s="32" t="s">
+        <v>18</v>
+      </c>
       <c r="B48" s="4" t="s">
-        <v>7</v>
+        <v>233</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="64"/>
+      <c r="A49" s="48"/>
       <c r="B49" s="4" t="s">
-        <v>200</v>
+        <v>234</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>77</v>
+        <v>238</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="64"/>
+      <c r="A50" s="48"/>
       <c r="B50" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>115</v>
@@ -2605,33 +2626,33 @@
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="47"/>
+      <c r="A51" s="48"/>
       <c r="B51" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>122</v>
+        <v>196</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
+      <c r="G51" s="4" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
-        <v>19</v>
-      </c>
+      <c r="A52" s="48"/>
       <c r="B52" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>115</v>
@@ -2639,16 +2660,16 @@
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
       <c r="G52" s="4" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
+      <c r="A53" s="33"/>
       <c r="B53" s="4" t="s">
         <v>138</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D53" s="15" t="s">
         <v>122</v>
@@ -2658,149 +2679,143 @@
       <c r="G53" s="4"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>31</v>
+      <c r="A54" s="50" t="s">
+        <v>19</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>78</v>
+        <v>231</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="E54" s="4"/>
-      <c r="F54" s="4">
-        <v>55</v>
-      </c>
-      <c r="G54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="A55" s="50"/>
       <c r="B55" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>71</v>
+        <v>138</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="E55" s="4"/>
-      <c r="F55" s="4">
-        <v>55</v>
-      </c>
+      <c r="F55" s="4"/>
       <c r="G55" s="4"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>154</v>
+        <v>78</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>156</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E56" s="4"/>
       <c r="F56" s="4">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="G56" s="4"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4">
+        <v>55</v>
+      </c>
+      <c r="G57" s="4"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F58" s="4">
+        <v>20</v>
+      </c>
+      <c r="G58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B59" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C59" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E59" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="D57" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F57" s="4">
+      <c r="F59" s="4">
         <v>21</v>
       </c>
-      <c r="G57" s="4"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="34" t="s">
+      <c r="G59" s="4"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B58" s="35"/>
-      <c r="C58" s="35"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="35"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="50" t="s">
-        <v>251</v>
-      </c>
-      <c r="I58" s="50"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="23" t="s">
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="41"/>
+      <c r="H60" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="I60" s="27"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="54" t="s">
         <v>139</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B61" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C59" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="D59" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="H59" t="s">
-        <v>254</v>
-      </c>
-      <c r="I59" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="24"/>
-      <c r="B60" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>150</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="24"/>
-      <c r="B61" s="13" t="s">
-        <v>8</v>
-      </c>
       <c r="C61" s="13" t="s">
-        <v>158</v>
+        <v>248</v>
       </c>
       <c r="D61" s="13" t="s">
         <v>115</v>
@@ -2808,177 +2823,177 @@
       <c r="E61" s="13"/>
       <c r="F61" s="13"/>
       <c r="G61" s="13" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+      <c r="H61" t="s">
+        <v>253</v>
+      </c>
+      <c r="I61" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="25"/>
+      <c r="A62" s="55"/>
       <c r="B62" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>122</v>
+        <v>7</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="E62" s="13"/>
       <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
+      <c r="G62" s="13" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="37" t="s">
+      <c r="A63" s="55"/>
+      <c r="B63" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="56"/>
+      <c r="B64" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="38"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="38"/>
-      <c r="F63" s="38"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="50" t="s">
-        <v>251</v>
-      </c>
-      <c r="I63" s="50"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="20" t="s">
+      <c r="B65" s="43"/>
+      <c r="C65" s="43"/>
+      <c r="D65" s="43"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="43"/>
+      <c r="G65" s="44"/>
+      <c r="H65" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="I65" s="27"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="51" t="s">
         <v>137</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B66" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="H64" t="s">
-        <v>257</v>
-      </c>
-      <c r="I64" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="21"/>
-      <c r="B65" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="16" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="21"/>
-      <c r="B66" s="14" t="s">
-        <v>8</v>
-      </c>
       <c r="C66" s="14" t="s">
-        <v>161</v>
+        <v>265</v>
       </c>
       <c r="D66" s="14" t="s">
         <v>115</v>
       </c>
       <c r="E66" s="14"/>
       <c r="F66" s="14"/>
-      <c r="G66" s="16" t="s">
-        <v>145</v>
+      <c r="G66" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="H66" t="s">
+        <v>256</v>
+      </c>
+      <c r="I66" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="22"/>
+      <c r="A67" s="52"/>
       <c r="B67" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C67" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D67" s="15" t="s">
-        <v>122</v>
+        <v>7</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>115</v>
       </c>
       <c r="E67" s="14"/>
       <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
+      <c r="G67" s="16" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="40" t="s">
+      <c r="A68" s="52"/>
+      <c r="B68" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="53"/>
+      <c r="B69" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="B68" s="41"/>
-      <c r="C68" s="41"/>
-      <c r="D68" s="41"/>
-      <c r="E68" s="41"/>
-      <c r="F68" s="41"/>
-      <c r="G68" s="42"/>
-      <c r="H68" s="50" t="s">
-        <v>251</v>
-      </c>
-      <c r="I68" s="50"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
+      <c r="B70" s="46"/>
+      <c r="C70" s="46"/>
+      <c r="D70" s="46"/>
+      <c r="E70" s="46"/>
+      <c r="F70" s="46"/>
+      <c r="G70" s="47"/>
+      <c r="H70" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="I70" s="27"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B71" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C69" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E69" s="6"/>
-      <c r="F69" s="6"/>
-      <c r="G69" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="H69" t="s">
-        <v>262</v>
-      </c>
-      <c r="I69" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="19"/>
-      <c r="B70" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E70" s="6"/>
-      <c r="F70" s="6"/>
-      <c r="G70" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="19"/>
-      <c r="B71" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="C71" s="6" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>115</v>
@@ -2986,33 +3001,39 @@
       <c r="E71" s="6"/>
       <c r="F71" s="6"/>
       <c r="G71" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H71" t="s">
+        <v>250</v>
+      </c>
+      <c r="I71" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="28"/>
+      <c r="B72" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="6" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="19"/>
-      <c r="B72" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C72" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="D72" s="15" t="s">
-        <v>122</v>
+      <c r="D72" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="E72" s="6"/>
       <c r="F72" s="6"/>
-      <c r="G72" s="6"/>
+      <c r="G72" s="6" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="19" t="s">
-        <v>37</v>
-      </c>
+      <c r="A73" s="28"/>
       <c r="B73" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>115</v>
@@ -3020,33 +3041,33 @@
       <c r="E73" s="6"/>
       <c r="F73" s="6"/>
       <c r="G73" s="6" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="19"/>
+      <c r="A74" s="28"/>
       <c r="B74" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>115</v>
+        <v>138</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
-      <c r="G74" s="6" t="s">
-        <v>170</v>
-      </c>
+      <c r="G74" s="6"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="19"/>
+      <c r="A75" s="28" t="s">
+        <v>37</v>
+      </c>
       <c r="B75" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>165</v>
+        <v>261</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>115</v>
@@ -3054,16 +3075,16 @@
       <c r="E75" s="6"/>
       <c r="F75" s="6"/>
       <c r="G75" s="6" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="19"/>
+      <c r="A76" s="28"/>
       <c r="B76" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>211</v>
+        <v>167</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>115</v>
@@ -3071,33 +3092,33 @@
       <c r="E76" s="6"/>
       <c r="F76" s="6"/>
       <c r="G76" s="6" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="19"/>
+      <c r="A77" s="28"/>
       <c r="B77" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C77" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="D77" s="15" t="s">
-        <v>122</v>
+        <v>8</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="E77" s="6"/>
       <c r="F77" s="6"/>
-      <c r="G77" s="6"/>
+      <c r="G77" s="6" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="19" t="s">
-        <v>38</v>
-      </c>
+      <c r="A78" s="28"/>
       <c r="B78" s="6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>169</v>
+        <v>207</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>115</v>
@@ -3105,33 +3126,33 @@
       <c r="E78" s="6"/>
       <c r="F78" s="6"/>
       <c r="G78" s="6" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="19"/>
+      <c r="A79" s="28"/>
       <c r="B79" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>115</v>
+        <v>61</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="E79" s="6"/>
       <c r="F79" s="6"/>
-      <c r="G79" s="6" t="s">
-        <v>178</v>
-      </c>
+      <c r="G79" s="6"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="19"/>
+      <c r="A80" s="28" t="s">
+        <v>38</v>
+      </c>
       <c r="B80" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>115</v>
@@ -3139,16 +3160,16 @@
       <c r="E80" s="6"/>
       <c r="F80" s="6"/>
       <c r="G80" s="6" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="19"/>
+      <c r="A81" s="28"/>
       <c r="B81" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>115</v>
@@ -3156,33 +3177,33 @@
       <c r="E81" s="6"/>
       <c r="F81" s="6"/>
       <c r="G81" s="6" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="19"/>
+      <c r="A82" s="28"/>
       <c r="B82" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="D82" s="15" t="s">
-        <v>122</v>
+        <v>8</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="E82" s="6"/>
       <c r="F82" s="6"/>
-      <c r="G82" s="6"/>
+      <c r="G82" s="6" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="19" t="s">
-        <v>39</v>
-      </c>
+      <c r="A83" s="28"/>
       <c r="B83" s="6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>115</v>
@@ -3190,33 +3211,33 @@
       <c r="E83" s="6"/>
       <c r="F83" s="6"/>
       <c r="G83" s="6" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="19"/>
+      <c r="A84" s="28"/>
       <c r="B84" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>115</v>
+        <v>61</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>122</v>
       </c>
       <c r="E84" s="6"/>
       <c r="F84" s="6"/>
-      <c r="G84" s="6" t="s">
-        <v>197</v>
-      </c>
+      <c r="G84" s="6"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="19"/>
+      <c r="A85" s="28" t="s">
+        <v>39</v>
+      </c>
       <c r="B85" s="6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="D85" s="6" t="s">
         <v>115</v>
@@ -3224,16 +3245,16 @@
       <c r="E85" s="6"/>
       <c r="F85" s="6"/>
       <c r="G85" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="19"/>
+      <c r="A86" s="28"/>
       <c r="B86" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>115</v>
@@ -3241,301 +3262,335 @@
       <c r="E86" s="6"/>
       <c r="F86" s="6"/>
       <c r="G86" s="6" t="s">
-        <v>153</v>
+        <v>193</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="19"/>
+      <c r="A87" s="28"/>
       <c r="B87" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C87" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="D87" s="15" t="s">
-        <v>122</v>
+        <v>8</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="E87" s="6"/>
       <c r="F87" s="6"/>
-      <c r="G87" s="6"/>
+      <c r="G87" s="6" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="26" t="s">
+      <c r="A88" s="28"/>
+      <c r="B88" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="28"/>
+      <c r="B89" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B88" s="27"/>
-      <c r="C88" s="27"/>
-      <c r="D88" s="27"/>
-      <c r="E88" s="27"/>
-      <c r="F88" s="27"/>
-      <c r="G88" s="28"/>
-      <c r="H88" s="50" t="s">
-        <v>251</v>
-      </c>
-      <c r="I88" s="50"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="17" t="s">
+      <c r="B90" s="58"/>
+      <c r="C90" s="58"/>
+      <c r="D90" s="58"/>
+      <c r="E90" s="58"/>
+      <c r="F90" s="58"/>
+      <c r="G90" s="59"/>
+      <c r="H90" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="I90" s="27"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B91" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
-      <c r="G89" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="H89" t="s">
-        <v>252</v>
-      </c>
-      <c r="I89" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="17"/>
-      <c r="B90" s="1" t="s">
+      <c r="C91" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="H91" t="s">
+        <v>246</v>
+      </c>
+      <c r="I91" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="49"/>
+      <c r="B92" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1" t="s">
+      <c r="C92" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="49"/>
+      <c r="B93" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="17"/>
-      <c r="B91" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D91" s="1" t="s">
+      <c r="C93" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D93" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1">
-        <v>55</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="17"/>
-      <c r="B92" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1">
-        <v>30</v>
-      </c>
-      <c r="G92" s="1"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="17"/>
-      <c r="B93" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="E93" s="1"/>
       <c r="F93" s="1">
+        <v>55</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="49"/>
+      <c r="B94" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E94" s="1"/>
+      <c r="F94" s="1">
+        <v>30</v>
+      </c>
+      <c r="G94" s="1"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="49"/>
+      <c r="B95" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E95" s="1"/>
+      <c r="F95" s="1">
         <v>31</v>
       </c>
-      <c r="G93" s="1"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="17"/>
-      <c r="B94" s="1" t="s">
+      <c r="G95" s="1"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="49"/>
+      <c r="B96" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C94" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="D94" s="15" t="s">
+      <c r="C96" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="D96" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F95" s="1">
-        <v>55</v>
-      </c>
-      <c r="G95" s="1"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E96" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F96" s="1">
-        <v>30</v>
-      </c>
+      <c r="E96" s="1"/>
+      <c r="F96" s="1"/>
       <c r="G96" s="1"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F97" s="1">
+        <v>55</v>
+      </c>
+      <c r="G97" s="1"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F98" s="1">
+        <v>30</v>
+      </c>
+      <c r="G98" s="1"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B99" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D97" s="1" t="s">
+      <c r="C99" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D99" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E97" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F97" s="1">
+      <c r="E99" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F99" s="1">
         <v>31</v>
       </c>
-      <c r="G97" s="1"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="43" t="s">
-        <v>219</v>
-      </c>
-      <c r="B98" s="44"/>
-      <c r="C98" s="44"/>
-      <c r="D98" s="44"/>
-      <c r="E98" s="44"/>
-      <c r="F98" s="44"/>
-      <c r="G98" s="45"/>
-      <c r="H98" s="50" t="s">
-        <v>251</v>
-      </c>
-      <c r="I98" s="50"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="46" t="s">
-        <v>192</v>
-      </c>
-      <c r="B99" s="4" t="s">
+      <c r="G99" s="1"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="B100" s="30"/>
+      <c r="C100" s="30"/>
+      <c r="D100" s="30"/>
+      <c r="E100" s="30"/>
+      <c r="F100" s="30"/>
+      <c r="G100" s="31"/>
+      <c r="H100" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="I100" s="27"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="B101" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C99" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D99" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E99" s="4"/>
-      <c r="F99" s="4"/>
-      <c r="G99" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="H99" t="s">
-        <v>220</v>
-      </c>
-      <c r="I99" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="47"/>
-      <c r="B100" s="4" t="s">
+      <c r="C101" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E101" s="4"/>
+      <c r="F101" s="4"/>
+      <c r="G101" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="H101" t="s">
+        <v>214</v>
+      </c>
+      <c r="I101" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="33"/>
+      <c r="B102" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C100" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="D100" s="15" t="s">
+      <c r="C102" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D102" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="E100" s="4"/>
-      <c r="F100" s="4"/>
-      <c r="G100" s="4"/>
+      <c r="E102" s="4"/>
+      <c r="F102" s="4"/>
+      <c r="G102" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="H98:I98"/>
-    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="A75:A79"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A90:G90"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="A80:A84"/>
+    <mergeCell ref="A85:A89"/>
+    <mergeCell ref="A100:G100"/>
+    <mergeCell ref="A101:A102"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="A70:G70"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="A48:A53"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="H100:I100"/>
+    <mergeCell ref="H70:I70"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="H88:I88"/>
-    <mergeCell ref="A78:A82"/>
-    <mergeCell ref="A83:A87"/>
-    <mergeCell ref="A98:G98"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A58:G58"/>
-    <mergeCell ref="A63:G63"/>
-    <mergeCell ref="A68:G68"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="A46:A51"/>
-    <mergeCell ref="A89:A94"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A18"/>
-    <mergeCell ref="A19:A24"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="A73:A77"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A88:G88"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="H90:I90"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3547,7 +3602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A44E18F-3292-4DA7-BDEA-F4A46B480A45}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -3746,31 +3801,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" style="51" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="19" customWidth="1"/>
     <col min="2" max="2" width="65.7109375" customWidth="1"/>
-    <col min="3" max="3" width="37" style="52" customWidth="1"/>
+    <col min="3" max="3" width="37" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55"/>
-      <c r="C1" s="56"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="63"/>
     </row>
     <row r="2" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="str">
+      <c r="A2" s="64" t="str">
         <f>IP!A3</f>
         <v>MSK-R14</v>
       </c>
-      <c r="B2" s="53" t="str">
+      <c r="B2" s="21" t="str">
         <f>"int "&amp;IP!B3&amp;CHAR(10)&amp;"ip address "&amp;IP!C3&amp;" "&amp;IP!D3&amp;CHAR(10)&amp;"description '"&amp;IP!G3&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/0
 ip address 10.0.254.12 255.255.255.254
 description 'to R12.e0/2'
 no shutdown</v>
       </c>
-      <c r="C2" s="58" t="str">
+      <c r="C2" s="60" t="str">
         <f>B2&amp;CHAR(10)&amp;B3&amp;CHAR(10)&amp;B4&amp;CHAR(10)&amp;B5&amp;CHAR(10)&amp;B6</f>
         <v>int e0/0
 ip address 10.0.254.12 255.255.255.254
@@ -3781,7 +3836,7 @@
 description 'to R13.e0/3'
 no shutdown
 int e0/2
-ip address 10.0.254.27 255.255.255.254
+ip address 10.0.254.17 255.255.255.254
 description 'to KTN-R22.e0/0'
 no shutdown
 int e0/3
@@ -3795,62 +3850,62 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="57"/>
-      <c r="B3" s="53" t="str">
+      <c r="A3" s="64"/>
+      <c r="B3" s="21" t="str">
         <f>"int "&amp;IP!B4&amp;CHAR(10)&amp;"ip address "&amp;IP!C4&amp;" "&amp;IP!D4&amp;CHAR(10)&amp;"description '"&amp;IP!G4&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/1
 ip address 10.0.254.2 255.255.255.254
 description 'to R13.e0/3'
 no shutdown</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="60"/>
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
-      <c r="B4" s="53" t="str">
+      <c r="A4" s="64"/>
+      <c r="B4" s="21" t="str">
         <f>"int "&amp;IP!B5&amp;CHAR(10)&amp;"ip address "&amp;IP!C5&amp;" "&amp;IP!D5&amp;CHAR(10)&amp;"description '"&amp;IP!G5&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/2
-ip address 10.0.254.27 255.255.255.254
+ip address 10.0.254.17 255.255.255.254
 description 'to KTN-R22.e0/0'
 no shutdown</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="60"/>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="57"/>
-      <c r="B5" s="53" t="str">
+      <c r="A5" s="64"/>
+      <c r="B5" s="21" t="str">
         <f>"int "&amp;IP!B6&amp;CHAR(10)&amp;"ip address "&amp;IP!C6&amp;" "&amp;IP!D6&amp;CHAR(10)&amp;"description '"&amp;IP!G6&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/3
 ip address 10.0.254.4 255.255.255.254
 description 'to R19.e0/0'
 no shutdown</v>
       </c>
-      <c r="C5" s="58"/>
+      <c r="C5" s="60"/>
     </row>
     <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57"/>
-      <c r="B6" s="53" t="str">
-        <f>"int "&amp;IP!B7&amp;CHAR(10)&amp;"ip address "&amp;IP!C7&amp;" "&amp;IP!D7&amp;CHAR(10)&amp;"description '"&amp;IP!G7&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A6" s="64"/>
+      <c r="B6" s="21" t="str">
+        <f>"int "&amp;IP!B8&amp;CHAR(10)&amp;"ip address "&amp;IP!C8&amp;" "&amp;IP!D8&amp;CHAR(10)&amp;"description '"&amp;IP!G8&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int lo
 ip address 172.16.255.14 255.255.255.255
 description ''
 no shutdown</v>
       </c>
-      <c r="C6" s="58"/>
+      <c r="C6" s="60"/>
     </row>
     <row r="7" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="str">
-        <f>IP!A8</f>
+      <c r="A7" s="64" t="str">
+        <f>IP!A9</f>
         <v>MSK-R15</v>
       </c>
-      <c r="B7" s="53" t="str">
-        <f>"int "&amp;IP!B8&amp;CHAR(10)&amp;"ip address "&amp;IP!C8&amp;" "&amp;IP!D8&amp;CHAR(10)&amp;"description '"&amp;IP!G8&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="B7" s="21" t="str">
+        <f>"int "&amp;IP!B9&amp;CHAR(10)&amp;"ip address "&amp;IP!C9&amp;" "&amp;IP!D9&amp;CHAR(10)&amp;"description '"&amp;IP!G9&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/0
 ip address 10.0.254.8 255.255.255.254
 description 'to R13.e0/2'
 no shutdown</v>
       </c>
-      <c r="C7" s="58" t="str">
+      <c r="C7" s="60" t="str">
         <f>B7&amp;CHAR(10)&amp;B8&amp;CHAR(10)&amp;B9&amp;CHAR(10)&amp;B10&amp;CHAR(10)&amp;B11</f>
         <v>int e0/0
 ip address 10.0.254.8 255.255.255.254
@@ -3875,62 +3930,62 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="57"/>
-      <c r="B8" s="53" t="str">
-        <f>"int "&amp;IP!B9&amp;CHAR(10)&amp;"ip address "&amp;IP!C9&amp;" "&amp;IP!D9&amp;CHAR(10)&amp;"description '"&amp;IP!G9&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A8" s="64"/>
+      <c r="B8" s="21" t="str">
+        <f>"int "&amp;IP!B10&amp;CHAR(10)&amp;"ip address "&amp;IP!C10&amp;" "&amp;IP!D10&amp;CHAR(10)&amp;"description '"&amp;IP!G10&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/1
 ip address 10.0.254.6 255.255.255.254
 description 'to R12.e0/3'
 no shutdown</v>
       </c>
-      <c r="C8" s="58"/>
+      <c r="C8" s="60"/>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="57"/>
-      <c r="B9" s="53" t="str">
-        <f>"int "&amp;IP!B10&amp;CHAR(10)&amp;"ip address "&amp;IP!C10&amp;" "&amp;IP!D10&amp;CHAR(10)&amp;"description '"&amp;IP!G10&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A9" s="64"/>
+      <c r="B9" s="21" t="str">
+        <f>"int "&amp;IP!B11&amp;CHAR(10)&amp;"ip address "&amp;IP!C11&amp;" "&amp;IP!D11&amp;CHAR(10)&amp;"description '"&amp;IP!G11&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/2
 ip address 10.0.254.19 255.255.255.254
 description 'to LMS-R21.e0/0'
 no shutdown</v>
       </c>
-      <c r="C9" s="58"/>
+      <c r="C9" s="60"/>
     </row>
     <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="57"/>
-      <c r="B10" s="53" t="str">
-        <f>"int "&amp;IP!B11&amp;CHAR(10)&amp;"ip address "&amp;IP!C11&amp;" "&amp;IP!D11&amp;CHAR(10)&amp;"description '"&amp;IP!G11&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A10" s="64"/>
+      <c r="B10" s="21" t="str">
+        <f>"int "&amp;IP!B12&amp;CHAR(10)&amp;"ip address "&amp;IP!C12&amp;" "&amp;IP!D12&amp;CHAR(10)&amp;"description '"&amp;IP!G12&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/3
 ip address 10.0.254.10 255.255.255.254
 description 'to R20.e0/0'
 no shutdown</v>
       </c>
-      <c r="C10" s="58"/>
+      <c r="C10" s="60"/>
     </row>
     <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="57"/>
-      <c r="B11" s="53" t="str">
-        <f>"int "&amp;IP!B12&amp;CHAR(10)&amp;"ip address "&amp;IP!C12&amp;" "&amp;IP!D12&amp;CHAR(10)&amp;"description '"&amp;IP!G12&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A11" s="64"/>
+      <c r="B11" s="21" t="str">
+        <f>"int "&amp;IP!B14&amp;CHAR(10)&amp;"ip address "&amp;IP!C14&amp;" "&amp;IP!D14&amp;CHAR(10)&amp;"description '"&amp;IP!G14&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int lo0
 ip address 172.16.255.15 255.255.255.0
 description ''
 no shutdown</v>
       </c>
-      <c r="C11" s="58"/>
+      <c r="C11" s="60"/>
     </row>
     <row r="12" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="57" t="str">
-        <f>IP!A13</f>
+      <c r="A12" s="64" t="str">
+        <f>IP!A15</f>
         <v>MSK-R12</v>
       </c>
-      <c r="B12" s="53" t="str">
-        <f>"int "&amp;IP!B13&amp;CHAR(10)&amp;"ip address "&amp;IP!C13&amp;" "&amp;IP!D13&amp;CHAR(10)&amp;"description '"&amp;IP!G13&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="B12" s="21" t="str">
+        <f>"int "&amp;IP!B15&amp;CHAR(10)&amp;"ip address "&amp;IP!C15&amp;" "&amp;IP!D15&amp;CHAR(10)&amp;"description '"&amp;IP!G15&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/0.10
 ip address 192.168.10.2 255.255.255.0
 description 'glpb 10 ip 192.168.10.1'
 no shutdown</v>
       </c>
-      <c r="C12" s="58" t="str">
+      <c r="C12" s="60" t="str">
         <f>B12&amp;CHAR(10)&amp;B13&amp;CHAR(10)&amp;B14&amp;CHAR(10)&amp;B15&amp;CHAR(10)&amp;B16&amp;CHAR(10)&amp;B17&amp;CHAR(10)</f>
         <v xml:space="preserve">int e0/0.10
 ip address 192.168.10.2 255.255.255.0
@@ -3960,73 +4015,73 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="57"/>
-      <c r="B13" s="53" t="str">
-        <f>"int "&amp;IP!B14&amp;CHAR(10)&amp;"ip address "&amp;IP!C14&amp;" "&amp;IP!D14&amp;CHAR(10)&amp;"description '"&amp;IP!G14&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A13" s="64"/>
+      <c r="B13" s="21" t="str">
+        <f>"int "&amp;IP!B16&amp;CHAR(10)&amp;"ip address "&amp;IP!C16&amp;" "&amp;IP!D16&amp;CHAR(10)&amp;"description '"&amp;IP!G16&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/0.11
 ip address 192.168.11.2 255.255.255.0
 description 'glpb 11 ip 192.168.11.1'
 no shutdown</v>
       </c>
-      <c r="C13" s="58"/>
+      <c r="C13" s="60"/>
     </row>
     <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
-      <c r="B14" s="53" t="str">
-        <f>"int "&amp;IP!B15&amp;CHAR(10)&amp;"ip address "&amp;IP!C15&amp;" "&amp;IP!D15&amp;CHAR(10)&amp;"description '"&amp;IP!G15&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A14" s="64"/>
+      <c r="B14" s="21" t="str">
+        <f>"int "&amp;IP!B17&amp;CHAR(10)&amp;"ip address "&amp;IP!C17&amp;" "&amp;IP!D17&amp;CHAR(10)&amp;"description '"&amp;IP!G17&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/1.55
 ip address 172.16.254.2 255.255.255.240
 description 'glpb 55 ip 172.16.254.1'
 no shutdown</v>
       </c>
-      <c r="C14" s="58"/>
+      <c r="C14" s="60"/>
     </row>
     <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="57"/>
-      <c r="B15" s="53" t="str">
-        <f>"int "&amp;IP!B16&amp;CHAR(10)&amp;"ip address "&amp;IP!C16&amp;" "&amp;IP!D16&amp;CHAR(10)&amp;"description '"&amp;IP!G16&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A15" s="64"/>
+      <c r="B15" s="21" t="str">
+        <f>"int "&amp;IP!B18&amp;CHAR(10)&amp;"ip address "&amp;IP!C18&amp;" "&amp;IP!D18&amp;CHAR(10)&amp;"description '"&amp;IP!G18&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/2
 ip address 10.0.254.13 255.255.255.254
 description 'to R14.e0/0'
 no shutdown</v>
       </c>
-      <c r="C15" s="58"/>
+      <c r="C15" s="60"/>
     </row>
     <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="57"/>
-      <c r="B16" s="53" t="str">
-        <f>"int "&amp;IP!B17&amp;CHAR(10)&amp;"ip address "&amp;IP!C17&amp;" "&amp;IP!D17&amp;CHAR(10)&amp;"description '"&amp;IP!G17&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A16" s="64"/>
+      <c r="B16" s="21" t="str">
+        <f>"int "&amp;IP!B19&amp;CHAR(10)&amp;"ip address "&amp;IP!C19&amp;" "&amp;IP!D19&amp;CHAR(10)&amp;"description '"&amp;IP!G19&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/3
 ip address 10.0.254.7 255.255.255.254
 description 'to R15.e0/1'
 no shutdown</v>
       </c>
-      <c r="C16" s="58"/>
+      <c r="C16" s="60"/>
     </row>
     <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="57"/>
-      <c r="B17" s="53" t="str">
-        <f>"int "&amp;IP!B18&amp;CHAR(10)&amp;"ip address "&amp;IP!C18&amp;" "&amp;IP!D18&amp;CHAR(10)&amp;"description '"&amp;IP!G18&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A17" s="64"/>
+      <c r="B17" s="21" t="str">
+        <f>"int "&amp;IP!B20&amp;CHAR(10)&amp;"ip address "&amp;IP!C20&amp;" "&amp;IP!D20&amp;CHAR(10)&amp;"description '"&amp;IP!G20&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int lo0
 ip address 172.16.255.12 255.255.255.255
 description ''
 no shutdown</v>
       </c>
-      <c r="C17" s="58"/>
+      <c r="C17" s="60"/>
     </row>
     <row r="18" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="57" t="str">
-        <f>IP!A19</f>
+      <c r="A18" s="64" t="str">
+        <f>IP!A21</f>
         <v>MSK-R13</v>
       </c>
-      <c r="B18" s="53" t="str">
-        <f>"int "&amp;IP!B19&amp;CHAR(10)&amp;"ip address "&amp;IP!C19&amp;" "&amp;IP!D19&amp;CHAR(10)&amp;"description '"&amp;IP!G19&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="B18" s="21" t="str">
+        <f>"int "&amp;IP!B21&amp;CHAR(10)&amp;"ip address "&amp;IP!C21&amp;" "&amp;IP!D21&amp;CHAR(10)&amp;"description '"&amp;IP!G21&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/0.10
 ip address 192.168.10.3 255.255.255.0
 description 'glpb 10 ip 192.168.10.1'
 no shutdown</v>
       </c>
-      <c r="C18" s="58" t="str">
+      <c r="C18" s="60" t="str">
         <f>B18&amp;CHAR(10)&amp;B19&amp;CHAR(10)&amp;B20&amp;CHAR(10)&amp;B21&amp;CHAR(10)&amp;B22&amp;CHAR(10)&amp;B23</f>
         <v>int e0/0.10
 ip address 192.168.10.3 255.255.255.0
@@ -4055,73 +4110,73 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="57"/>
-      <c r="B19" s="53" t="str">
-        <f>"int "&amp;IP!B20&amp;CHAR(10)&amp;"ip address "&amp;IP!C20&amp;" "&amp;IP!D20&amp;CHAR(10)&amp;"description '"&amp;IP!G20&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A19" s="64"/>
+      <c r="B19" s="21" t="str">
+        <f>"int "&amp;IP!B22&amp;CHAR(10)&amp;"ip address "&amp;IP!C22&amp;" "&amp;IP!D22&amp;CHAR(10)&amp;"description '"&amp;IP!G22&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/0.11
 ip address 192.168.11.3 255.255.255.0
 description 'glpb 11 ip 192.168.11.1'
 no shutdown</v>
       </c>
-      <c r="C19" s="58"/>
+      <c r="C19" s="60"/>
     </row>
     <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="57"/>
-      <c r="B20" s="53" t="str">
-        <f>"int "&amp;IP!B21&amp;CHAR(10)&amp;"ip address "&amp;IP!C21&amp;" "&amp;IP!D21&amp;CHAR(10)&amp;"description '"&amp;IP!G21&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A20" s="64"/>
+      <c r="B20" s="21" t="str">
+        <f>"int "&amp;IP!B23&amp;CHAR(10)&amp;"ip address "&amp;IP!C23&amp;" "&amp;IP!D23&amp;CHAR(10)&amp;"description '"&amp;IP!G23&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/1.55
 ip address 172.16.254.3 255.255.255.240
 description 'glpb 55 ip 172.16.254.1'
 no shutdown</v>
       </c>
-      <c r="C20" s="58"/>
+      <c r="C20" s="60"/>
     </row>
     <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="57"/>
-      <c r="B21" s="53" t="str">
-        <f>"int "&amp;IP!B22&amp;CHAR(10)&amp;"ip address "&amp;IP!C22&amp;" "&amp;IP!D22&amp;CHAR(10)&amp;"description '"&amp;IP!G22&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A21" s="64"/>
+      <c r="B21" s="21" t="str">
+        <f>"int "&amp;IP!B24&amp;CHAR(10)&amp;"ip address "&amp;IP!C24&amp;" "&amp;IP!D24&amp;CHAR(10)&amp;"description '"&amp;IP!G24&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/2
 ip address 10.0.254.9 255.255.255.254
 description 'to R15.e0/0'
 no shutdown</v>
       </c>
-      <c r="C21" s="58"/>
+      <c r="C21" s="60"/>
     </row>
     <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="57"/>
-      <c r="B22" s="53" t="str">
-        <f>"int "&amp;IP!B23&amp;CHAR(10)&amp;"ip address "&amp;IP!C23&amp;" "&amp;IP!D23&amp;CHAR(10)&amp;"description '"&amp;IP!G23&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A22" s="64"/>
+      <c r="B22" s="21" t="str">
+        <f>"int "&amp;IP!B25&amp;CHAR(10)&amp;"ip address "&amp;IP!C25&amp;" "&amp;IP!D25&amp;CHAR(10)&amp;"description '"&amp;IP!G25&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/3
 ip address 10.0.254.3 255.255.255.254
 description 'to R14.e0/1'
 no shutdown</v>
       </c>
-      <c r="C22" s="58"/>
+      <c r="C22" s="60"/>
     </row>
     <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="57"/>
-      <c r="B23" s="53" t="str">
-        <f>"int "&amp;IP!B24&amp;CHAR(10)&amp;"ip address "&amp;IP!C24&amp;" "&amp;IP!D24&amp;CHAR(10)&amp;"description '"&amp;IP!G24&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A23" s="64"/>
+      <c r="B23" s="21" t="str">
+        <f>"int "&amp;IP!B26&amp;CHAR(10)&amp;"ip address "&amp;IP!C26&amp;" "&amp;IP!D26&amp;CHAR(10)&amp;"description '"&amp;IP!G26&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int lo0
 ip address 172.16.255.13 255.255.255.255
 description ''
 no shutdown</v>
       </c>
-      <c r="C23" s="58"/>
+      <c r="C23" s="60"/>
     </row>
     <row r="24" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="57" t="str">
-        <f>IP!A25</f>
+      <c r="A24" s="64" t="str">
+        <f>IP!A27</f>
         <v>MSK-R19</v>
       </c>
-      <c r="B24" s="53" t="str">
-        <f>"int "&amp;IP!B25&amp;CHAR(10)&amp;"ip address "&amp;IP!C25&amp;" "&amp;IP!D25&amp;CHAR(10)&amp;"description '"&amp;IP!G25&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="B24" s="21" t="str">
+        <f>"int "&amp;IP!B27&amp;CHAR(10)&amp;"ip address "&amp;IP!C27&amp;" "&amp;IP!D27&amp;CHAR(10)&amp;"description '"&amp;IP!G27&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/0
 ip address 10.0.254.5 255.255.255.254
 description 'to R14.e0/3'
 no shutdown</v>
       </c>
-      <c r="C24" s="58" t="str">
+      <c r="C24" s="60" t="str">
         <f>"hostname "&amp;A24&amp;CHAR(10)&amp;B24&amp;CHAR(10)&amp;B25</f>
         <v>hostname MSK-R19
 int e0/0
@@ -4135,29 +4190,29 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="57"/>
-      <c r="B25" s="53" t="str">
-        <f>"int "&amp;IP!B26&amp;CHAR(10)&amp;"ip address "&amp;IP!C26&amp;" "&amp;IP!D26&amp;CHAR(10)&amp;"description '"&amp;IP!G26&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A25" s="64"/>
+      <c r="B25" s="21" t="str">
+        <f>"int "&amp;IP!B28&amp;CHAR(10)&amp;"ip address "&amp;IP!C28&amp;" "&amp;IP!D28&amp;CHAR(10)&amp;"description '"&amp;IP!G28&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int lo0
 ip address 172.16.255.19 255.255.255.255
 description ''
 no shutdown</v>
       </c>
-      <c r="C25" s="58"/>
+      <c r="C25" s="60"/>
     </row>
     <row r="26" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="57" t="str">
-        <f>IP!A27</f>
+      <c r="A26" s="64" t="str">
+        <f>IP!A29</f>
         <v>MSK-R20</v>
       </c>
-      <c r="B26" s="53" t="str">
-        <f>"int "&amp;IP!B27&amp;CHAR(10)&amp;"ip address "&amp;IP!C27&amp;" "&amp;IP!D27&amp;CHAR(10)&amp;"description '"&amp;IP!G27&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="B26" s="21" t="str">
+        <f>"int "&amp;IP!B29&amp;CHAR(10)&amp;"ip address "&amp;IP!C29&amp;" "&amp;IP!D29&amp;CHAR(10)&amp;"description '"&amp;IP!G29&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int e0/0
 ip address 10.0.254.11 255.255.255.254
 description 'to R15.e0/3'
 no shutdown</v>
       </c>
-      <c r="C26" s="58" t="str">
+      <c r="C26" s="60" t="str">
         <f>"hostname "&amp;A26&amp;CHAR(10)&amp;B26&amp;CHAR(10)&amp;B27</f>
         <v>hostname MSK-R20
 int e0/0
@@ -4171,29 +4226,29 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="57"/>
-      <c r="B27" s="53" t="str">
-        <f>"int "&amp;IP!B28&amp;CHAR(10)&amp;"ip address "&amp;IP!C28&amp;" "&amp;IP!D28&amp;CHAR(10)&amp;"description '"&amp;IP!G28&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="A27" s="64"/>
+      <c r="B27" s="21" t="str">
+        <f>"int "&amp;IP!B30&amp;CHAR(10)&amp;"ip address "&amp;IP!C30&amp;" "&amp;IP!D30&amp;CHAR(10)&amp;"description '"&amp;IP!G30&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int lo0
 ip address 172.16.255.20 255.255.255.255
 description ''
 no shutdown</v>
       </c>
-      <c r="C27" s="58"/>
+      <c r="C27" s="60"/>
     </row>
     <row r="28" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="59" t="str">
-        <f>IP!A29</f>
+      <c r="A28" s="22" t="str">
+        <f>IP!A31</f>
         <v>MSK-SW4</v>
       </c>
-      <c r="B28" s="53" t="str">
-        <f>"int "&amp;IP!B29&amp;CHAR(10)&amp;"ip address "&amp;IP!C29&amp;" "&amp;IP!D29&amp;CHAR(10)&amp;"description '"&amp;IP!G29&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="B28" s="21" t="str">
+        <f>"int "&amp;IP!B31&amp;CHAR(10)&amp;"ip address "&amp;IP!C31&amp;" "&amp;IP!D31&amp;CHAR(10)&amp;"description '"&amp;IP!G31&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int vlan55
 ip address 172.16.254.6 255.255.255.240
 description ''
 no shutdown</v>
       </c>
-      <c r="C28" s="60" t="str">
+      <c r="C28" s="23" t="str">
         <f t="shared" ref="C28:C29" si="0">B28</f>
         <v>int vlan55
 ip address 172.16.254.6 255.255.255.240
@@ -4202,18 +4257,18 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="59" t="str">
-        <f>IP!A30</f>
+      <c r="A29" s="22" t="str">
+        <f>IP!A32</f>
         <v>MSK-SW5</v>
       </c>
-      <c r="B29" s="53" t="str">
-        <f>"int "&amp;IP!B30&amp;CHAR(10)&amp;"ip address "&amp;IP!C30&amp;" "&amp;IP!D30&amp;CHAR(10)&amp;"description '"&amp;IP!G30&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="B29" s="21" t="str">
+        <f>"int "&amp;IP!B32&amp;CHAR(10)&amp;"ip address "&amp;IP!C32&amp;" "&amp;IP!D32&amp;CHAR(10)&amp;"description '"&amp;IP!G32&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int vlan55
 ip address 172.16.254.7 255.255.255.240
 description ''
 no shutdown</v>
       </c>
-      <c r="C29" s="60" t="str">
+      <c r="C29" s="23" t="str">
         <f t="shared" si="0"/>
         <v>int vlan55
 ip address 172.16.254.7 255.255.255.240
@@ -4222,18 +4277,18 @@
       </c>
     </row>
     <row r="30" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="59" t="str">
-        <f>IP!A31</f>
+      <c r="A30" s="22" t="str">
+        <f>IP!A33</f>
         <v>MSK-SW2</v>
       </c>
-      <c r="B30" s="53" t="str">
-        <f>"int "&amp;IP!B31&amp;CHAR(10)&amp;"ip address "&amp;IP!C31&amp;" "&amp;IP!D31&amp;CHAR(10)&amp;"description '"&amp;IP!G31&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="B30" s="21" t="str">
+        <f>"int "&amp;IP!B33&amp;CHAR(10)&amp;"ip address "&amp;IP!C33&amp;" "&amp;IP!D33&amp;CHAR(10)&amp;"description '"&amp;IP!G33&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int vlan55
 ip address 172.16.254.8 255.255.255.240
 description ''
 no shutdown</v>
       </c>
-      <c r="C30" s="60" t="str">
+      <c r="C30" s="23" t="str">
         <f>B30</f>
         <v>int vlan55
 ip address 172.16.254.8 255.255.255.240
@@ -4242,18 +4297,18 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="61" t="str">
-        <f>IP!A32</f>
+      <c r="A31" s="24" t="str">
+        <f>IP!A34</f>
         <v>MSK-SW3</v>
       </c>
-      <c r="B31" s="62" t="str">
-        <f>"int "&amp;IP!B32&amp;CHAR(10)&amp;"ip address "&amp;IP!C32&amp;" "&amp;IP!D32&amp;CHAR(10)&amp;"description '"&amp;IP!G32&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
+      <c r="B31" s="25" t="str">
+        <f>"int "&amp;IP!B34&amp;CHAR(10)&amp;"ip address "&amp;IP!C34&amp;" "&amp;IP!D34&amp;CHAR(10)&amp;"description '"&amp;IP!G34&amp;"'"&amp;CHAR(10)&amp;"no shutdown"</f>
         <v>int vlan55
 ip address 172.16.254.9 255.255.255.240
 description ''
 no shutdown</v>
       </c>
-      <c r="C31" s="63" t="str">
+      <c r="C31" s="26" t="str">
         <f>B31</f>
         <v>int vlan55
 ip address 172.16.254.9 255.255.255.240
@@ -4338,276 +4393,271 @@
       <c r="C98"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="49"/>
+      <c r="B99" s="18"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="49"/>
+      <c r="B100" s="18"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B101" s="49"/>
+      <c r="B101" s="18"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="49"/>
+      <c r="B102" s="18"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="49"/>
+      <c r="B103" s="18"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="49"/>
+      <c r="B104" s="18"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="49"/>
+      <c r="B105" s="18"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B106" s="49"/>
+      <c r="B106" s="18"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="49"/>
+      <c r="B107" s="18"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="49"/>
+      <c r="B108" s="18"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B109" s="49"/>
+      <c r="B109" s="18"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B110" s="49"/>
+      <c r="B110" s="18"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B111" s="49"/>
+      <c r="B111" s="18"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B112" s="49"/>
+      <c r="B112" s="18"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B113" s="49"/>
+      <c r="B113" s="18"/>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="49"/>
+      <c r="B114" s="18"/>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="49"/>
+      <c r="B115" s="18"/>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="49"/>
+      <c r="B116" s="18"/>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="49"/>
+      <c r="B117" s="18"/>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B118" s="49"/>
+      <c r="B118" s="18"/>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B119" s="49"/>
+      <c r="B119" s="18"/>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B120" s="49"/>
+      <c r="B120" s="18"/>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="49"/>
+      <c r="B121" s="18"/>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="49"/>
+      <c r="B122" s="18"/>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B123" s="49"/>
+      <c r="B123" s="18"/>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B124" s="49"/>
+      <c r="B124" s="18"/>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B125" s="49"/>
+      <c r="B125" s="18"/>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="49"/>
+      <c r="B126" s="18"/>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="49"/>
+      <c r="B127" s="18"/>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B128" s="49"/>
+      <c r="B128" s="18"/>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B129" s="49"/>
+      <c r="B129" s="18"/>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B130" s="49"/>
+      <c r="B130" s="18"/>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="49"/>
+      <c r="B131" s="18"/>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="49"/>
+      <c r="B132" s="18"/>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B133" s="49"/>
+      <c r="B133" s="18"/>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B134" s="49"/>
+      <c r="B134" s="18"/>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B135" s="49"/>
+      <c r="B135" s="18"/>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="49"/>
+      <c r="B136" s="18"/>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="49"/>
+      <c r="B137" s="18"/>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="49"/>
+      <c r="B138" s="18"/>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="49"/>
+      <c r="B139" s="18"/>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="49"/>
+      <c r="B140" s="18"/>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="49"/>
+      <c r="B141" s="18"/>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="49"/>
+      <c r="B142" s="18"/>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B143" s="49"/>
+      <c r="B143" s="18"/>
     </row>
     <row r="144" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B144" s="49"/>
+      <c r="B144" s="18"/>
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B145" s="49"/>
+      <c r="B145" s="18"/>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B146" s="49"/>
+      <c r="B146" s="18"/>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B147" s="49"/>
+      <c r="B147" s="18"/>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B148" s="49"/>
+      <c r="B148" s="18"/>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B149" s="49"/>
+      <c r="B149" s="18"/>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="49"/>
+      <c r="B150" s="18"/>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="49"/>
+      <c r="B151" s="18"/>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B152" s="49"/>
+      <c r="B152" s="18"/>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="49"/>
+      <c r="B153" s="18"/>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="49"/>
+      <c r="B154" s="18"/>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155" s="49"/>
+      <c r="B155" s="18"/>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156" s="49"/>
+      <c r="B156" s="18"/>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B157" s="49"/>
+      <c r="B157" s="18"/>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B158" s="49"/>
+      <c r="B158" s="18"/>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B159" s="49"/>
+      <c r="B159" s="18"/>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="49"/>
+      <c r="B160" s="18"/>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B161" s="49"/>
+      <c r="B161" s="18"/>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B162" s="49"/>
+      <c r="B162" s="18"/>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B163" s="49"/>
+      <c r="B163" s="18"/>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164" s="49"/>
+      <c r="B164" s="18"/>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B165" s="49"/>
+      <c r="B165" s="18"/>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B166" s="49"/>
+      <c r="B166" s="18"/>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B167" s="49"/>
+      <c r="B167" s="18"/>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B168" s="49"/>
+      <c r="B168" s="18"/>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B169" s="49"/>
+      <c r="B169" s="18"/>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B170" s="49"/>
+      <c r="B170" s="18"/>
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B171" s="49"/>
+      <c r="B171" s="18"/>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B172" s="49"/>
+      <c r="B172" s="18"/>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B173" s="49"/>
+      <c r="B173" s="18"/>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B174" s="49"/>
+      <c r="B174" s="18"/>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B175" s="49"/>
+      <c r="B175" s="18"/>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B176" s="49"/>
+      <c r="B176" s="18"/>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B177" s="49"/>
+      <c r="B177" s="18"/>
     </row>
     <row r="178" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B178" s="49"/>
+      <c r="B178" s="18"/>
     </row>
     <row r="179" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B179" s="49"/>
+      <c r="B179" s="18"/>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B180" s="49"/>
+      <c r="B180" s="18"/>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B181" s="49"/>
+      <c r="B181" s="18"/>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B182" s="49"/>
+      <c r="B182" s="18"/>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B183" s="49"/>
+      <c r="B183" s="18"/>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B184" s="49"/>
+      <c r="B184" s="18"/>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B185" s="49"/>
+      <c r="B185" s="18"/>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B186" s="49"/>
+      <c r="B186" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C12:C17"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="C18:C23"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="A2:A6"/>
@@ -4616,6 +4666,11 @@
     <mergeCell ref="A18:A23"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
+    <mergeCell ref="C12:C17"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="C18:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>